<commit_message>
the final modification made by my self
</commit_message>
<xml_diff>
--- a/figures/bufopt.xlsx
+++ b/figures/bufopt.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <r>
       <t>f</t>
@@ -80,6 +80,12 @@
       </rPr>
       <t>4</t>
     </r>
+  </si>
+  <si>
+    <t>LLBA</t>
+  </si>
+  <si>
+    <t>our method</t>
   </si>
 </sst>
 </file>
@@ -638,11 +644,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="156822528"/>
-        <c:axId val="128367936"/>
+        <c:axId val="115358720"/>
+        <c:axId val="95868544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156822528"/>
+        <c:axId val="115358720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,7 +677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128367936"/>
+        <c:crossAx val="95868544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -679,7 +685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128367936"/>
+        <c:axId val="95868544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,7 +715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156822528"/>
+        <c:crossAx val="115358720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -742,10 +748,373 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:effectLst>
+      <a:glow>
+        <a:schemeClr val="accent1">
+          <a:alpha val="40000"/>
+        </a:schemeClr>
+      </a:glow>
+    </a:effectLst>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LLBA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$18:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>our method</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$18:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57777777777777772</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57777777777777772</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48888888888888887</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48888888888888887</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48888888888888887</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48888888888888887</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1456128"/>
+        <c:axId val="108159552"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1456128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Deadline constraint (cycles)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108159552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="108159552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Normalized buffer requirement</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1456128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22955621172353455"/>
+          <c:y val="3.6653178769320505E-2"/>
+          <c:w val="0.35933267716535433"/>
+          <c:h val="0.16743438320209975"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -755,15 +1124,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -777,6 +1146,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1072,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1296,6 +1695,206 @@
       </c>
       <c r="E13">
         <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f>G18/45</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="G18">
+        <f>SUM(B2:E2)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E29" si="0">G19/45</f>
+        <v>0.68888888888888888</v>
+      </c>
+      <c r="G19">
+        <f>SUM(B3:E3)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="G20">
+        <f>SUM(B4:E4)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="G21">
+        <f>SUM(B5:E5)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G22">
+        <f>SUM(B6:E6)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G23">
+        <f>SUM(B7:E7)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="G24">
+        <f>SUM(B8:E8)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="G25">
+        <f>SUM(B9:E9)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26">
+        <v>46</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="G26">
+        <f>SUM(B10:E10)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="G27">
+        <f>SUM(B11:E11)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G28">
+        <f>SUM(B12:E12)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29">
+        <v>52</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G29">
+        <f>SUM(B13:E13)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>